<commit_message>
updated case studies, test_strategic_model, and model doc
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elmira\Documents\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A907BF1C-0BB0-41FC-9141-036D9496699C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721232A6-DD46-47CA-A599-FBD24BF2F9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="834" firstSheet="62" activeTab="68" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="834" firstSheet="64" activeTab="68" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -37989,7 +37989,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38018,7 +38018,7 @@
         <v>140</v>
       </c>
       <c r="C3" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38029,7 +38029,7 @@
         <v>140</v>
       </c>
       <c r="C4" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38040,7 +38040,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38051,7 +38051,7 @@
         <v>140</v>
       </c>
       <c r="C6" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38062,7 +38062,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38073,7 +38073,7 @@
         <v>141</v>
       </c>
       <c r="C8" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38084,7 +38084,7 @@
         <v>141</v>
       </c>
       <c r="C9" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38095,7 +38095,7 @@
         <v>141</v>
       </c>
       <c r="C10" s="34">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38106,7 +38106,7 @@
         <v>142</v>
       </c>
       <c r="C11" s="34">
-        <v>0.9</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38117,7 +38117,7 @@
         <v>142</v>
       </c>
       <c r="C12" s="34">
-        <v>0.9</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38128,7 +38128,7 @@
         <v>142</v>
       </c>
       <c r="C13" s="34">
-        <v>0.9</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
@@ -38139,7 +38139,7 @@
         <v>142</v>
       </c>
       <c r="C14" s="35">
-        <v>0.9</v>
+        <v>0.995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add config argument for removal efficiency calculation method
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elmira\Documents\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721232A6-DD46-47CA-A599-FBD24BF2F9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E40309-BD57-4E11-AA92-FA1E145F5B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="834" firstSheet="64" activeTab="68" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -37989,7 +37989,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38018,7 +38018,7 @@
         <v>140</v>
       </c>
       <c r="C3" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38029,7 +38029,7 @@
         <v>140</v>
       </c>
       <c r="C4" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38040,7 +38040,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38051,7 +38051,7 @@
         <v>140</v>
       </c>
       <c r="C6" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38062,7 +38062,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38073,7 +38073,7 @@
         <v>141</v>
       </c>
       <c r="C8" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38084,7 +38084,7 @@
         <v>141</v>
       </c>
       <c r="C9" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38095,7 +38095,7 @@
         <v>141</v>
       </c>
       <c r="C10" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38106,7 +38106,7 @@
         <v>142</v>
       </c>
       <c r="C11" s="34">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38117,7 +38117,7 @@
         <v>142</v>
       </c>
       <c r="C12" s="34">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38128,7 +38128,7 @@
         <v>142</v>
       </c>
       <c r="C13" s="34">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
@@ -38139,7 +38139,7 @@
         <v>142</v>
       </c>
       <c r="C14" s="35">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test for both removal efficiency config, revised small case study, revised documentation
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elmira\Documents\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E40309-BD57-4E11-AA92-FA1E145F5B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80DDBD0-DB78-4E46-9CB2-9D9AC27E7140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="834" firstSheet="64" activeTab="68" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -987,7 +987,7 @@
     <t>Table with indication if the treatment technology is for desalination</t>
   </si>
   <si>
-    <t>Table of Removal Efficiency [%]</t>
+    <t>Table of Removal Efficiency [%]. Note: The removal efficiency of a component can be estimated based on its concentration or its total load (flow times concentration). The default method for calculating removal efficacy is concentration-based. This configuration option is set prior to running the optimization. Refer to 'Water Treatment' in Model Library documentation.</t>
   </si>
 </sst>
 </file>
@@ -37989,7 +37989,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
add config argument for removal efficiency calculation method (#228)
* add config argument for removal efficiency calculation method

* change water_quality argument to false

* changed water_quality to false

* added test for both removal efficiency config, revised small case study, revised documentation

* renamed quality test functions for clarity

* applied black
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elmira\Documents\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721232A6-DD46-47CA-A599-FBD24BF2F9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80DDBD0-DB78-4E46-9CB2-9D9AC27E7140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="834" firstSheet="64" activeTab="68" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -987,7 +987,7 @@
     <t>Table with indication if the treatment technology is for desalination</t>
   </si>
   <si>
-    <t>Table of Removal Efficiency [%]</t>
+    <t>Table of Removal Efficiency [%]. Note: The removal efficiency of a component can be estimated based on its concentration or its total load (flow times concentration). The default method for calculating removal efficacy is concentration-based. This configuration option is set prior to running the optimization. Refer to 'Water Treatment' in Model Library documentation.</t>
   </si>
 </sst>
 </file>
@@ -37989,7 +37989,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -38018,7 +38018,7 @@
         <v>140</v>
       </c>
       <c r="C3" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38029,7 +38029,7 @@
         <v>140</v>
       </c>
       <c r="C4" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38040,7 +38040,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38051,7 +38051,7 @@
         <v>140</v>
       </c>
       <c r="C6" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38062,7 +38062,7 @@
         <v>141</v>
       </c>
       <c r="C7" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38073,7 +38073,7 @@
         <v>141</v>
       </c>
       <c r="C8" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38084,7 +38084,7 @@
         <v>141</v>
       </c>
       <c r="C9" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38095,7 +38095,7 @@
         <v>141</v>
       </c>
       <c r="C10" s="34">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38106,7 +38106,7 @@
         <v>142</v>
       </c>
       <c r="C11" s="34">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38117,7 +38117,7 @@
         <v>142</v>
       </c>
       <c r="C12" s="34">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.3" x14ac:dyDescent="0.55000000000000004">
@@ -38128,7 +38128,7 @@
         <v>142</v>
       </c>
       <c r="C13" s="34">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" thickBot="1" x14ac:dyDescent="0.6">
@@ -38139,7 +38139,7 @@
         <v>142</v>
       </c>
       <c r="C14" s="35">
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update permian demo input file
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pareto\source_code\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662E691B-8AF0-47A4-AE0B-FDF2AB98D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B946B7-D77B-4DB0-BAE1-6B46278508A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="834" firstSheet="17" activeTab="43" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="5985" yWindow="3105" windowWidth="28800" windowHeight="15195" tabRatio="834" activeTab="2" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -7431,7 +7431,7 @@
   </sheetPr>
   <dimension ref="A1:BA12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:K9"/>
     </sheetView>
   </sheetViews>
@@ -24688,7 +24688,7 @@
   </sheetPr>
   <dimension ref="A1:BF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
add post-optimization timing calculation for storage, disposal, pipelines
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4802EF38-2C00-44E5-AB4C-B585E220B4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE910DB5-83DB-4511-A87A-154FCC1DFEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="834" firstSheet="75" activeTab="82" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="79" activeTab="84" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -96,7 +96,8 @@
     <sheet name="TreatmentExpansionLeadTime" sheetId="121" r:id="rId81"/>
     <sheet name="DisposalExpansionLeadTime" sheetId="122" r:id="rId82"/>
     <sheet name="StorageExpansionLeadTime" sheetId="123" r:id="rId83"/>
-    <sheet name="PipelineExpansionLeadTime" sheetId="120" r:id="rId84"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="120" r:id="rId84"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="124" r:id="rId85"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="66" hidden="1">#REF!</definedName>
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3402" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="308">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1044,6 +1045,9 @@
   </si>
   <si>
     <t>Table of Production Rate Forecasts by Pads [bbl/day]</t>
+  </si>
+  <si>
+    <t>pipeline_expansion_lead_time</t>
   </si>
 </sst>
 </file>
@@ -6944,7 +6948,7 @@
   <dimension ref="A1:BA12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -38401,9 +38405,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -38448,7 +38450,7 @@
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5:E6"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30:XFD30"/>
+      <selection pane="bottomLeft" activeCell="AQ49" sqref="AQ49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44574,7 +44576,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45838,7 +45840,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46218,16 +46220,16 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time [",VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"s]")</f>
-        <v>Table of Storage Expansion Lead Time [days]</v>
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"s]")</f>
+        <v>Table of Pipeline Expansion Lead Time - Distance Based [days]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -46286,12 +46288,152 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"s/",VLOOKUP("distance", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Pipeline Expansion Lead Time - Distance Based [days/mile]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="39">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E435A8-16A8-45F0-B48E-2BA75B04538C}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"s]")</f>
+        <v>Table of Pipeline Expansion Lead Time - Distance Based [days]</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="52">
+        <v>30</v>
+      </c>
+      <c r="D3" s="52">
+        <v>30</v>
+      </c>
+      <c r="E3" s="53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="52">
+        <v>30</v>
+      </c>
+      <c r="D4" s="52">
+        <v>30</v>
+      </c>
+      <c r="E4" s="53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="52">
+        <v>30</v>
+      </c>
+      <c r="D5" s="52">
+        <v>30</v>
+      </c>
+      <c r="E5" s="53">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="55">
+        <v>30</v>
+      </c>
+      <c r="D6" s="55">
+        <v>30</v>
+      </c>
+      <c r="E6" s="56">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add new tabs to all case study files, update to realistic values
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15788C23-7E82-480E-AB85-C4C72ABB0817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68331FA3-B4C3-4919-9323-B9DF25A0542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="929" firstSheet="87" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-1740" windowWidth="29040" windowHeight="17640" tabRatio="929" firstSheet="87" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1701,7 +1701,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2008,6 +2008,10 @@
     <xf numFmtId="3" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2227,8 +2231,8 @@
       <sheetName val="PipelineExpansionLeadTime_Capac"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
@@ -2311,88 +2315,88 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+      <sheetData sheetId="61" refreshError="1"/>
+      <sheetData sheetId="62" refreshError="1"/>
+      <sheetData sheetId="63" refreshError="1"/>
+      <sheetData sheetId="64" refreshError="1"/>
+      <sheetData sheetId="65" refreshError="1"/>
+      <sheetData sheetId="66" refreshError="1"/>
+      <sheetData sheetId="67" refreshError="1"/>
+      <sheetData sheetId="68" refreshError="1"/>
+      <sheetData sheetId="69" refreshError="1"/>
+      <sheetData sheetId="70" refreshError="1"/>
+      <sheetData sheetId="71" refreshError="1"/>
+      <sheetData sheetId="72" refreshError="1"/>
+      <sheetData sheetId="73" refreshError="1"/>
+      <sheetData sheetId="74" refreshError="1"/>
+      <sheetData sheetId="75" refreshError="1"/>
+      <sheetData sheetId="76" refreshError="1"/>
+      <sheetData sheetId="77" refreshError="1"/>
+      <sheetData sheetId="78" refreshError="1"/>
+      <sheetData sheetId="79" refreshError="1"/>
+      <sheetData sheetId="80" refreshError="1"/>
+      <sheetData sheetId="81" refreshError="1"/>
+      <sheetData sheetId="82" refreshError="1"/>
+      <sheetData sheetId="83" refreshError="1"/>
+      <sheetData sheetId="84" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3261,7 +3265,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -38501,7 +38505,7 @@
   <dimension ref="A1:AR56"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A13" sqref="A13"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
@@ -45929,8 +45933,8 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45974,16 +45978,16 @@
         <v>140</v>
       </c>
       <c r="C3" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D3" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E3" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F3" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -45994,16 +45998,16 @@
         <v>140</v>
       </c>
       <c r="C4" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D4" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E4" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F4" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46014,16 +46018,16 @@
         <v>140</v>
       </c>
       <c r="C5" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D5" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E5" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F5" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46034,16 +46038,16 @@
         <v>140</v>
       </c>
       <c r="C6" s="130">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D6" s="116">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E6" s="116">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F6" s="84">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46054,16 +46058,16 @@
         <v>141</v>
       </c>
       <c r="C7" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D7" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E7" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F7" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46074,16 +46078,16 @@
         <v>141</v>
       </c>
       <c r="C8" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D8" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E8" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F8" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46094,16 +46098,16 @@
         <v>141</v>
       </c>
       <c r="C9" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D9" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E9" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F9" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46114,16 +46118,16 @@
         <v>141</v>
       </c>
       <c r="C10" s="130">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D10" s="116">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E10" s="116">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F10" s="84">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46134,16 +46138,16 @@
         <v>142</v>
       </c>
       <c r="C11" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D11" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E11" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F11" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46154,16 +46158,16 @@
         <v>142</v>
       </c>
       <c r="C12" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D12" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E12" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F12" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -46174,16 +46178,16 @@
         <v>142</v>
       </c>
       <c r="C13" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D13" s="36">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E13" s="36">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F13" s="37">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -46194,16 +46198,16 @@
         <v>142</v>
       </c>
       <c r="C14" s="38">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D14" s="38">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="E14" s="38">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="F14" s="39">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -46218,8 +46222,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46248,10 +46252,10 @@
         <v>123</v>
       </c>
       <c r="B3" s="131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C3" s="37">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -46259,10 +46263,10 @@
         <v>124</v>
       </c>
       <c r="B4" s="131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C4" s="37">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -46270,10 +46274,10 @@
         <v>125</v>
       </c>
       <c r="B5" s="131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C5" s="37">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -46281,10 +46285,10 @@
         <v>126</v>
       </c>
       <c r="B6" s="131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C6" s="37">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -46292,10 +46296,10 @@
         <v>127</v>
       </c>
       <c r="B7" s="38">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C7" s="39">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -46310,8 +46314,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46340,10 +46344,10 @@
         <v>132</v>
       </c>
       <c r="B3" s="131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C3" s="37">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -46351,10 +46355,10 @@
         <v>133</v>
       </c>
       <c r="B4" s="131">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C4" s="37">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -46362,10 +46366,10 @@
         <v>134</v>
       </c>
       <c r="B5" s="38">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C5" s="39">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -46380,8 +46384,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46407,8 +46411,8 @@
       <c r="A3" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="B3" s="39">
-        <v>30</v>
+      <c r="B3" s="132">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -46424,7 +46428,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46462,14 +46466,14 @@
       <c r="B3" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="52">
-        <v>30</v>
-      </c>
-      <c r="D3" s="52">
-        <v>30</v>
+      <c r="C3" s="133">
+        <v>0</v>
+      </c>
+      <c r="D3" s="133">
+        <v>1</v>
       </c>
       <c r="E3" s="53">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -46479,14 +46483,14 @@
       <c r="B4" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="52">
-        <v>30</v>
-      </c>
-      <c r="D4" s="52">
-        <v>30</v>
+      <c r="C4" s="133">
+        <v>0</v>
+      </c>
+      <c r="D4" s="133">
+        <v>1</v>
       </c>
       <c r="E4" s="53">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -46496,14 +46500,14 @@
       <c r="B5" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="52">
-        <v>30</v>
-      </c>
-      <c r="D5" s="52">
-        <v>30</v>
+      <c r="C5" s="133">
+        <v>0</v>
+      </c>
+      <c r="D5" s="133">
+        <v>1</v>
       </c>
       <c r="E5" s="53">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -46514,13 +46518,13 @@
         <v>153</v>
       </c>
       <c r="C6" s="55">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D6" s="55">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E6" s="56">
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolve remaining broken links
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520F04E9-BC1C-4212-92E3-79288104FB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E17D4-A77A-412F-908D-9D8F75C60A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="929" firstSheet="89" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="929" firstSheet="89" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -46050,8 +46050,8 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time - Distance Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Storage Expansion Lead Time - Distance Based [weeks]</v>
+        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
+        <v>Table of Storage Expansion Lead Time [weeks]</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>

<commit_message>
Implement beneficial reuse processing cost
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E855CB8A-D94C-4C9E-9995-A09D78048264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060E00B6-171A-4C7F-B650-B6F222ED2899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -97,18 +97,19 @@
     <sheet name="RemovalEfficiency" sheetId="114" r:id="rId82"/>
     <sheet name="DesalinationTechnologies" sheetId="111" r:id="rId83"/>
     <sheet name="DesalinationSites" sheetId="113" r:id="rId84"/>
-    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId85"/>
-    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId86"/>
-    <sheet name="Hydraulics" sheetId="93" r:id="rId87"/>
-    <sheet name="Economics" sheetId="95" r:id="rId88"/>
-    <sheet name="PadWaterQuality" sheetId="99" r:id="rId89"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId90"/>
-    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId91"/>
-    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId92"/>
-    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId93"/>
-    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId94"/>
-    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId95"/>
-    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId96"/>
+    <sheet name="BeneficialReuseCost" sheetId="138" r:id="rId85"/>
+    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId86"/>
+    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId87"/>
+    <sheet name="Hydraulics" sheetId="93" r:id="rId88"/>
+    <sheet name="Economics" sheetId="95" r:id="rId89"/>
+    <sheet name="PadWaterQuality" sheetId="99" r:id="rId90"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId91"/>
+    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId92"/>
+    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId93"/>
+    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId94"/>
+    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId95"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId96"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId97"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
@@ -45213,6 +45214,33 @@
 </file>
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823AFEBC-B792-4B8A-886B-A98A6A68E8F9}">
+  <sheetPr>
+    <tabColor rgb="FFAFF3DE"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>CONCATENATE( "Table with processing cost for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table with processing cost for sending water to beneficial reuse [USD/bbl]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6590066-9C40-4D54-9CAB-C4CFCBEB3031}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45220,7 +45248,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -45239,7 +45267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2338A37-BF8E-46F2-AA7C-FB95F874D0FC}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45298,7 +45326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDDE38-2D71-4494-ABC1-8D5269A138D9}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45372,7 +45400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45420,178 +45448,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134045F2-617D-4B6C-9AE3-C6E73CF3B321}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="B2" s="57" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="59">
-        <v>142277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="60">
-        <v>140998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="60">
-        <v>172490.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="60">
-        <v>257547</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="60">
-        <v>241833.8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="60">
-        <v>188503.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="60">
-        <v>146716</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="60">
-        <v>216563</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="60">
-        <v>150626</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="60">
-        <v>247061</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="60">
-        <v>180968</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="60">
-        <v>195584</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="60">
-        <v>148655</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="83" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="129">
-        <v>185369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="60">
-        <v>165376</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="61">
-        <v>240977</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -45649,6 +45505,178 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134045F2-617D-4B6C-9AE3-C6E73CF3B321}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="59">
+        <v>142277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="60">
+        <v>140998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="60">
+        <v>172490.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="60">
+        <v>257547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="60">
+        <v>241833.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="60">
+        <v>188503.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="60">
+        <v>146716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="60">
+        <v>216563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="60">
+        <v>150626</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="60">
+        <v>247061</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="60">
+        <v>180968</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="60">
+        <v>195584</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="60">
+        <v>148655</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="129">
+        <v>185369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="60">
+        <v>165376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="61">
+        <v>240977</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE4BAFD-2A94-4164-976F-B9E5B42E5AAB}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -45710,7 +45738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA334136-9628-4654-B8E2-BCFE701B0D1B}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -45763,7 +45791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF02372-561D-40F0-A559-919B07A104BB}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46052,7 +46080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFFE531-B1A6-4FB1-B54F-4F29B07D584D}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46144,7 +46172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB6A12E-8B05-4366-A90E-CF297972EC8F}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46214,7 +46242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE98AFE6-8AD4-4F61-8FD9-8C39A28FF436}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46257,7 +46285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64191092-61FC-49E2-8B87-F024EB93CA2E}">
   <sheetPr>
     <tabColor theme="0"/>

</xml_diff>

<commit_message>
add environmental objective, add units to environmental parameters and variables, update summary report to include costs when using alternative objectives
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A793C9-CDAD-47AC-9FAC-61498B5FC21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E17D4-A77A-412F-908D-9D8F75C60A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="929" firstSheet="88" activeTab="89" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="929" firstSheet="89" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -102,13 +102,11 @@
     <sheet name="PadWaterQuality" sheetId="99" r:id="rId87"/>
     <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId88"/>
     <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId89"/>
-    <sheet name="AirEmissionCoefficients" sheetId="134" r:id="rId90"/>
-    <sheet name="TreatmentEmissionCoefficients" sheetId="135" r:id="rId91"/>
-    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId92"/>
-    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId93"/>
-    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId94"/>
-    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId95"/>
-    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId96"/>
+    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId90"/>
+    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId91"/>
+    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId92"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId93"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId94"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="74" hidden="1">#REF!</definedName>
@@ -135,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3432" uniqueCount="314">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1078,36 +1076,6 @@
   <si>
     <t>pipeline_expansion_lead_time</t>
   </si>
-  <si>
-    <t>CO2</t>
-  </si>
-  <si>
-    <t>NH3</t>
-  </si>
-  <si>
-    <t>NOx</t>
-  </si>
-  <si>
-    <t>SO2</t>
-  </si>
-  <si>
-    <t>PM 2.5</t>
-  </si>
-  <si>
-    <t>Trucking (g/hour)</t>
-  </si>
-  <si>
-    <t>Pipeline Operations (g/(bbl-mile))</t>
-  </si>
-  <si>
-    <t>Pipeline Installation (g/mile)</t>
-  </si>
-  <si>
-    <t>Disposal (g/bbl)</t>
-  </si>
-  <si>
-    <t>Storage (g/bbl-week)</t>
-  </si>
 </sst>
 </file>
 
@@ -1212,7 +1180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1723,19 +1691,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1743,7 +1698,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2048,27 +2003,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -45721,270 +45655,6 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD14726F-A828-41EA-8E78-20C9A2A31A3F}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="62.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Air Emissions Coefficients ")</f>
-        <v xml:space="preserve">Table of Air Emissions Coefficients </v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C2" s="112" t="s">
-        <v>315</v>
-      </c>
-      <c r="D2" s="112" t="s">
-        <v>316</v>
-      </c>
-      <c r="E2" s="112" t="s">
-        <v>317</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
-        <v>319</v>
-      </c>
-      <c r="B3" s="132">
-        <v>2035000</v>
-      </c>
-      <c r="C3" s="132">
-        <v>35.75</v>
-      </c>
-      <c r="D3" s="132">
-        <v>12649.999999999998</v>
-      </c>
-      <c r="E3" s="132">
-        <v>770.00000000000011</v>
-      </c>
-      <c r="F3" s="132">
-        <v>120.99999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
-        <v>320</v>
-      </c>
-      <c r="B4" s="132">
-        <v>22</v>
-      </c>
-      <c r="C4" s="132">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="D4" s="132">
-        <v>1.4E-2</v>
-      </c>
-      <c r="E4" s="132">
-        <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="F4" s="133">
-        <v>8.5999999999999998E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="B5" s="132">
-        <v>310000000</v>
-      </c>
-      <c r="C5" s="132">
-        <v>2800</v>
-      </c>
-      <c r="D5" s="132">
-        <v>190000</v>
-      </c>
-      <c r="E5" s="132">
-        <v>100000</v>
-      </c>
-      <c r="F5" s="133">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="B6" s="132">
-        <v>970</v>
-      </c>
-      <c r="C6" s="132">
-        <v>0.13</v>
-      </c>
-      <c r="D6" s="132">
-        <v>9.5</v>
-      </c>
-      <c r="E6" s="132">
-        <v>2.8</v>
-      </c>
-      <c r="F6" s="133">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="B7" s="134">
-        <v>1000</v>
-      </c>
-      <c r="C7" s="134">
-        <v>1.2E-2</v>
-      </c>
-      <c r="D7" s="134">
-        <v>2</v>
-      </c>
-      <c r="E7" s="134">
-        <v>0.65</v>
-      </c>
-      <c r="F7" s="135">
-        <v>7.5999999999999998E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD4DC5B-96A4-4920-A58A-08D189576A6D}">
-  <sheetPr>
-    <tabColor theme="8" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Air Emissions Coefficients  for Treatment Technologies [emissions/volume time]")</f>
-        <v>Table of Air Emissions Coefficients  for Treatment Technologies [emissions/volume time]</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="136" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" s="112" t="s">
-        <v>314</v>
-      </c>
-      <c r="C2" s="112" t="s">
-        <v>315</v>
-      </c>
-      <c r="D2" s="112" t="s">
-        <v>316</v>
-      </c>
-      <c r="E2" s="112" t="s">
-        <v>317</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="137" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="132">
-        <v>9600</v>
-      </c>
-      <c r="C3" s="132">
-        <v>1.45</v>
-      </c>
-      <c r="D3" s="132">
-        <v>12.8</v>
-      </c>
-      <c r="E3" s="132">
-        <v>13.5</v>
-      </c>
-      <c r="F3" s="133">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="137" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="132">
-        <v>9600</v>
-      </c>
-      <c r="C4" s="132">
-        <v>1.45</v>
-      </c>
-      <c r="D4" s="132">
-        <v>12.8</v>
-      </c>
-      <c r="E4" s="132">
-        <v>13.5</v>
-      </c>
-      <c r="F4" s="133">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="138" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="134">
-        <v>9600</v>
-      </c>
-      <c r="C5" s="134">
-        <v>1.45</v>
-      </c>
-      <c r="D5" s="134">
-        <v>12.8</v>
-      </c>
-      <c r="E5" s="134">
-        <v>13.5</v>
-      </c>
-      <c r="F5" s="135">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF02372-561D-40F0-A559-919B07A104BB}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46273,7 +45943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFFE531-B1A6-4FB1-B54F-4F29B07D584D}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46365,7 +46035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB6A12E-8B05-4366-A90E-CF297972EC8F}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46435,7 +46105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE98AFE6-8AD4-4F61-8FD9-8C39A28FF436}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46478,14 +46148,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64191092-61FC-49E2-8B87-F024EB93CA2E}">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Implement water quality for freshwater sources
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060E00B6-171A-4C7F-B650-B6F222ED2899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF12496-C7D1-4B19-BBDD-1A29A3A5C4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -21,99 +21,101 @@
     <sheet name="CompletionsPads" sheetId="3" r:id="rId6"/>
     <sheet name="SWDSites" sheetId="4" r:id="rId7"/>
     <sheet name="FreshwaterSources" sheetId="35" r:id="rId8"/>
-    <sheet name="StorageSites" sheetId="36" r:id="rId9"/>
-    <sheet name="TreatmentSites" sheetId="37" r:id="rId10"/>
-    <sheet name="TreatmentTechnologies" sheetId="104" r:id="rId11"/>
-    <sheet name="ReuseOptions" sheetId="38" r:id="rId12"/>
-    <sheet name="NetworkNodes" sheetId="39" r:id="rId13"/>
-    <sheet name="PipelineDiameters" sheetId="53" r:id="rId14"/>
-    <sheet name="StorageCapacities" sheetId="54" r:id="rId15"/>
-    <sheet name="TreatmentCapacities" sheetId="86" r:id="rId16"/>
-    <sheet name="InjectionCapacities" sheetId="55" r:id="rId17"/>
-    <sheet name="PNA" sheetId="56" r:id="rId18"/>
-    <sheet name="CNA" sheetId="57" r:id="rId19"/>
-    <sheet name="CCA" sheetId="73" r:id="rId20"/>
-    <sheet name="NNA" sheetId="58" r:id="rId21"/>
-    <sheet name="NCA" sheetId="59" r:id="rId22"/>
-    <sheet name="NKA" sheetId="60" r:id="rId23"/>
-    <sheet name="NRA" sheetId="61" r:id="rId24"/>
-    <sheet name="NSA" sheetId="76" r:id="rId25"/>
-    <sheet name="NOA" sheetId="122" r:id="rId26"/>
-    <sheet name="SNA" sheetId="77" r:id="rId27"/>
-    <sheet name="SOA" sheetId="121" r:id="rId28"/>
-    <sheet name="FCA" sheetId="41" r:id="rId29"/>
-    <sheet name="RCA" sheetId="83" r:id="rId30"/>
-    <sheet name="RSA" sheetId="105" r:id="rId31"/>
-    <sheet name="SCA" sheetId="108" r:id="rId32"/>
-    <sheet name="RNA" sheetId="62" r:id="rId33"/>
-    <sheet name="ROA" sheetId="120" r:id="rId34"/>
-    <sheet name="RKA" sheetId="136" r:id="rId35"/>
-    <sheet name="PCT" sheetId="42" r:id="rId36"/>
-    <sheet name="FCT" sheetId="70" r:id="rId37"/>
-    <sheet name="PKT" sheetId="43" r:id="rId38"/>
-    <sheet name="CKT" sheetId="44" r:id="rId39"/>
-    <sheet name="CCT" sheetId="74" r:id="rId40"/>
-    <sheet name="CST" sheetId="64" r:id="rId41"/>
-    <sheet name="RST" sheetId="123" r:id="rId42"/>
-    <sheet name="ROT" sheetId="124" r:id="rId43"/>
-    <sheet name="SOT" sheetId="125" r:id="rId44"/>
-    <sheet name="RKT" sheetId="137" r:id="rId45"/>
-    <sheet name="Elevation" sheetId="115" r:id="rId46"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId47"/>
-    <sheet name="PadRates" sheetId="65" r:id="rId48"/>
-    <sheet name="FlowbackRates" sheetId="75" r:id="rId49"/>
-    <sheet name="WellPressure" sheetId="116" r:id="rId50"/>
-    <sheet name="InitialPipelineCapacity" sheetId="118" r:id="rId51"/>
-    <sheet name="InitialPipelineDiameters" sheetId="119" r:id="rId52"/>
-    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId53"/>
-    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId54"/>
-    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId55"/>
-    <sheet name="ReuseMinimum" sheetId="126" r:id="rId56"/>
-    <sheet name="ReuseCapacity" sheetId="127" r:id="rId57"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId58"/>
-    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId59"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId60"/>
-    <sheet name="NodeCapacities" sheetId="102" r:id="rId61"/>
-    <sheet name="DisposalOperatingCapacity" sheetId="112" r:id="rId62"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId63"/>
-    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId64"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId65"/>
-    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId66"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId67"/>
-    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId68"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId69"/>
-    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId70"/>
-    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId71"/>
-    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId72"/>
-    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId73"/>
-    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId74"/>
-    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId75"/>
-    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId76"/>
-    <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId77"/>
-    <sheet name="PipelineCapexCapacityBased" sheetId="98" r:id="rId78"/>
-    <sheet name="PipelineCapacityIncrements" sheetId="97" r:id="rId79"/>
-    <sheet name="PipelineDiameterValues" sheetId="78" r:id="rId80"/>
-    <sheet name="TreatmentEfficiency" sheetId="107" r:id="rId81"/>
-    <sheet name="RemovalEfficiency" sheetId="114" r:id="rId82"/>
-    <sheet name="DesalinationTechnologies" sheetId="111" r:id="rId83"/>
-    <sheet name="DesalinationSites" sheetId="113" r:id="rId84"/>
-    <sheet name="BeneficialReuseCost" sheetId="138" r:id="rId85"/>
-    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId86"/>
-    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId87"/>
-    <sheet name="Hydraulics" sheetId="93" r:id="rId88"/>
-    <sheet name="Economics" sheetId="95" r:id="rId89"/>
-    <sheet name="PadWaterQuality" sheetId="99" r:id="rId90"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId91"/>
-    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId92"/>
-    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId93"/>
-    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId94"/>
-    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId95"/>
-    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId96"/>
-    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId97"/>
+    <sheet name="WaterQualityComponents" sheetId="139" r:id="rId9"/>
+    <sheet name="StorageSites" sheetId="36" r:id="rId10"/>
+    <sheet name="TreatmentSites" sheetId="37" r:id="rId11"/>
+    <sheet name="TreatmentTechnologies" sheetId="104" r:id="rId12"/>
+    <sheet name="ReuseOptions" sheetId="38" r:id="rId13"/>
+    <sheet name="NetworkNodes" sheetId="39" r:id="rId14"/>
+    <sheet name="PipelineDiameters" sheetId="53" r:id="rId15"/>
+    <sheet name="StorageCapacities" sheetId="54" r:id="rId16"/>
+    <sheet name="TreatmentCapacities" sheetId="86" r:id="rId17"/>
+    <sheet name="InjectionCapacities" sheetId="55" r:id="rId18"/>
+    <sheet name="PNA" sheetId="56" r:id="rId19"/>
+    <sheet name="CNA" sheetId="57" r:id="rId20"/>
+    <sheet name="CCA" sheetId="73" r:id="rId21"/>
+    <sheet name="NNA" sheetId="58" r:id="rId22"/>
+    <sheet name="NCA" sheetId="59" r:id="rId23"/>
+    <sheet name="NKA" sheetId="60" r:id="rId24"/>
+    <sheet name="NRA" sheetId="61" r:id="rId25"/>
+    <sheet name="NSA" sheetId="76" r:id="rId26"/>
+    <sheet name="NOA" sheetId="122" r:id="rId27"/>
+    <sheet name="SNA" sheetId="77" r:id="rId28"/>
+    <sheet name="SOA" sheetId="121" r:id="rId29"/>
+    <sheet name="FCA" sheetId="41" r:id="rId30"/>
+    <sheet name="RCA" sheetId="83" r:id="rId31"/>
+    <sheet name="RSA" sheetId="105" r:id="rId32"/>
+    <sheet name="SCA" sheetId="108" r:id="rId33"/>
+    <sheet name="RNA" sheetId="62" r:id="rId34"/>
+    <sheet name="ROA" sheetId="120" r:id="rId35"/>
+    <sheet name="RKA" sheetId="136" r:id="rId36"/>
+    <sheet name="PCT" sheetId="42" r:id="rId37"/>
+    <sheet name="FCT" sheetId="70" r:id="rId38"/>
+    <sheet name="PKT" sheetId="43" r:id="rId39"/>
+    <sheet name="CKT" sheetId="44" r:id="rId40"/>
+    <sheet name="CCT" sheetId="74" r:id="rId41"/>
+    <sheet name="CST" sheetId="64" r:id="rId42"/>
+    <sheet name="RST" sheetId="123" r:id="rId43"/>
+    <sheet name="ROT" sheetId="124" r:id="rId44"/>
+    <sheet name="SOT" sheetId="125" r:id="rId45"/>
+    <sheet name="RKT" sheetId="137" r:id="rId46"/>
+    <sheet name="Elevation" sheetId="115" r:id="rId47"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId48"/>
+    <sheet name="PadRates" sheetId="65" r:id="rId49"/>
+    <sheet name="FlowbackRates" sheetId="75" r:id="rId50"/>
+    <sheet name="WellPressure" sheetId="116" r:id="rId51"/>
+    <sheet name="InitialPipelineCapacity" sheetId="118" r:id="rId52"/>
+    <sheet name="InitialPipelineDiameters" sheetId="119" r:id="rId53"/>
+    <sheet name="InitialDisposalCapacity" sheetId="46" r:id="rId54"/>
+    <sheet name="InitialStorageCapacity" sheetId="80" r:id="rId55"/>
+    <sheet name="InitialTreatmentCapacity" sheetId="67" r:id="rId56"/>
+    <sheet name="ReuseMinimum" sheetId="126" r:id="rId57"/>
+    <sheet name="ReuseCapacity" sheetId="127" r:id="rId58"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId59"/>
+    <sheet name="CompletionsPadStorage" sheetId="72" r:id="rId60"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId61"/>
+    <sheet name="NodeCapacities" sheetId="102" r:id="rId62"/>
+    <sheet name="DisposalOperatingCapacity" sheetId="112" r:id="rId63"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId64"/>
+    <sheet name="TreatmentOperationalCost" sheetId="68" r:id="rId65"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId66"/>
+    <sheet name="PipelineOperationalCost" sheetId="69" r:id="rId67"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId68"/>
+    <sheet name="TruckingHourlyCost" sheetId="71" r:id="rId69"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId70"/>
+    <sheet name="DisposalExpansionCost" sheetId="90" r:id="rId71"/>
+    <sheet name="DisposalCapacityIncrements" sheetId="79" r:id="rId72"/>
+    <sheet name="StorageExpansionCost" sheetId="91" r:id="rId73"/>
+    <sheet name="StorageCapacityIncrements" sheetId="81" r:id="rId74"/>
+    <sheet name="TreatmentExpansionCost" sheetId="92" r:id="rId75"/>
+    <sheet name="TreatmentCapacityIncrements" sheetId="87" r:id="rId76"/>
+    <sheet name="PipelineCapexDistanceBased" sheetId="89" r:id="rId77"/>
+    <sheet name="PipelineExpansionDistance" sheetId="94" r:id="rId78"/>
+    <sheet name="PipelineCapexCapacityBased" sheetId="98" r:id="rId79"/>
+    <sheet name="PipelineCapacityIncrements" sheetId="97" r:id="rId80"/>
+    <sheet name="PipelineDiameterValues" sheetId="78" r:id="rId81"/>
+    <sheet name="TreatmentEfficiency" sheetId="107" r:id="rId82"/>
+    <sheet name="RemovalEfficiency" sheetId="114" r:id="rId83"/>
+    <sheet name="DesalinationTechnologies" sheetId="111" r:id="rId84"/>
+    <sheet name="DesalinationSites" sheetId="113" r:id="rId85"/>
+    <sheet name="BeneficialReuseCost" sheetId="138" r:id="rId86"/>
+    <sheet name="BeneficialReuseCredit" sheetId="128" r:id="rId87"/>
+    <sheet name="CompletionsPadOutsideSystem" sheetId="110" r:id="rId88"/>
+    <sheet name="Hydraulics" sheetId="93" r:id="rId89"/>
+    <sheet name="Economics" sheetId="95" r:id="rId90"/>
+    <sheet name="FreshwaterQuality" sheetId="140" r:id="rId91"/>
+    <sheet name="PadWaterQuality" sheetId="99" r:id="rId92"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId93"/>
+    <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId94"/>
+    <sheet name="TreatmentExpansionLeadTime" sheetId="129" r:id="rId95"/>
+    <sheet name="DisposalExpansionLeadTime" sheetId="130" r:id="rId96"/>
+    <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId97"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId98"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId99"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="76">PipelineExpansionDistance!$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="77" hidden="1">#REF!</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="77">PipelineExpansionDistance!$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -136,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3440" uniqueCount="316">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1707,7 +1709,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2012,6 +2014,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2995,6 +3003,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3056,7 +3117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C820352-28DB-4692-BCE8-9A9846CC4956}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3112,7 +3173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3156,7 +3217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3338,7 +3399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E58F52A-57D4-400C-9B2D-0CDF39E9349F}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3388,7 +3449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153D1DC6-FF6C-4D1F-9E23-B1795807F580}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3448,7 +3509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A75646C-6D5B-41D2-BD66-0AABE8C35A83}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3512,7 +3573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E691EF25-02B9-4EAE-A04E-51FF0E4ADDCA}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3572,7 +3633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EADE56A-3552-4283-86E6-D2B76E77A8C0}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -4184,7 +4245,79 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F319BCD0-9FF0-4128-B77A-FE703C6CAEA8}">
+  <sheetPr>
+    <tabColor theme="2" tint="-9.9978637043366805E-2"/>
+  </sheetPr>
+  <dimension ref="C3:M36"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="40"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C21" s="41"/>
+      <c r="F21" s="41"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C23" s="42"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C24" s="42"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C25" s="42"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C26" s="42"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C27" s="42"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C28" s="42"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C29" s="42"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C30" s="42"/>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C31" s="42"/>
+      <c r="M31" s="26"/>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C32" s="42"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="42"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="42"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="42"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B44EC57-024F-431A-B1C2-58810C4F9E47}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -4409,79 +4542,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F319BCD0-9FF0-4128-B77A-FE703C6CAEA8}">
-  <sheetPr>
-    <tabColor theme="2" tint="-9.9978637043366805E-2"/>
-  </sheetPr>
-  <dimension ref="C3:M36"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="40"/>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="41"/>
-      <c r="F21" s="41"/>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C23" s="42"/>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="42"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C25" s="42"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="42"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="42"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="42"/>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="42"/>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C30" s="42"/>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="42"/>
-      <c r="M31" s="26"/>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="42"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="42"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="42"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="42"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="42"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F10C60C-760C-4F1B-AB9A-B14851122200}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -4547,7 +4608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399EB22-0DA7-4F9B-9913-FB50F464ABD0}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -5757,7 +5818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037676BC-0D9E-4EC2-B7DF-9077076036FD}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6029,7 +6090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B147A77C-3EC6-43F3-933A-7BFD421AB782}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6380,7 +6441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928AC5F8-3DBD-4182-95AF-F72C7FA4D2FF}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6693,7 +6754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A514516D-9002-4617-9A63-E1CA29CE5849}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6743,7 +6804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128C9F10-CE90-494D-8C57-8F92F1447238}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6799,7 +6860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E548F62-97B3-424F-8681-D1975DE263A9}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6853,7 +6914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5202470E-E975-4217-A409-8C10C569162A}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -6892,68 +6953,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7344,6 +7343,68 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05F6C2E-9295-44C7-B492-F6D27B8F0C30}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7418,7 +7479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E0DBD1-9C53-4E86-8483-588C08719311}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7497,7 +7558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E8874E-11ED-45FA-AE95-642AF80BF911}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7568,7 +7629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3F673B-ABE6-40C2-BA6B-F7AEA69D03F8}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7663,7 +7724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C95F9C-FA1A-429C-94DB-7469B7607C89}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7714,7 +7775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C390631-9141-4367-876C-8B8C7DB728DE}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7765,7 +7826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7920,7 +7981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F615298C-1D1C-4004-91BA-05C3C07D8B7C}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -7981,7 +8042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8300,114 +8361,6 @@
         <v>1</v>
       </c>
       <c r="F16" s="11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9">
-        <v>1</v>
-      </c>
-      <c r="F3" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1</v>
-      </c>
-      <c r="F4" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1</v>
-      </c>
-      <c r="C5" s="10">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="11">
         <v>1</v>
       </c>
     </row>
@@ -8524,6 +8477,114 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37622F2B-1E4B-46C9-B210-3150CCBB5892}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8589,7 +8650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A52059-0CB1-474F-ACFF-2997470BE1E9}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8631,7 +8692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C8D473-2930-44EE-8137-39B9510AF450}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8704,7 +8765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A0C474-4CA3-482D-8EF9-161A6D97C2DB}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8754,7 +8815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80EBF5B-386F-48FB-AEF9-824F4D45CD63}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8795,7 +8856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0760AB0-D32B-4E99-8ACD-C8EA595D930F}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -8845,7 +8906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70C2981-7DF6-4E1E-9B3F-307C90704C6F}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -9361,7 +9422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -10038,7 +10099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -12496,7 +12557,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68666333-AE69-4574-92B2-6BE3A00DF612}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -13037,113 +13204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675FE18E-3C30-49FC-B6A0-0A6D3F02EBB0}">
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4E79A3-EE1E-46A1-84CE-D8C5F14D9087}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -16682,7 +16743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F279D59-CF57-42CD-9C09-61C92D7047B6}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -24024,7 +24085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4083B03F-43EE-4FD3-B5B4-0D52688676BC}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -31353,7 +31414,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -31431,7 +31492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDF796A-A87C-4F37-A825-AF0AD18C802A}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -31492,7 +31553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A13F53-E3AE-452E-A1A1-316A2C800322}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -31591,7 +31652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6AC10C-C440-4ADB-A331-07AA535B16B7}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -31618,7 +31679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38BD3B1-CE73-47E8-BFE4-E0C0165A2C32}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -31645,7 +31706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -32278,68 +32339,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Pad Storage Capacity [bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="39">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -32400,6 +32399,68 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAB793D-71C1-4CA2-A5D0-D94D2FB81D42}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Completions Pad Storage Capacity [bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="39">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -32452,7 +32513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF13C221-12DF-4609-BB39-C92B41E7288D}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -32662,7 +32723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{938F1661-765C-4FF3-9C8D-056B836A43E1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -33671,7 +33732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -33749,7 +33810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7050C77-5C7B-4C97-8F2B-C60EA6AF1AED}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -33922,7 +33983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -33983,7 +34044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE24AD9-42B2-417F-BF2D-D0F067DA599C}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -36932,7 +36993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -36985,7 +37046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35585569-7889-4883-A327-3B12D4AB6358}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -37169,393 +37230,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:F19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="9">
-        <v>3</v>
-      </c>
-      <c r="C3" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="D3" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="E3" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="F3" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="C4" s="9">
-        <v>2</v>
-      </c>
-      <c r="D4" s="9">
-        <v>5</v>
-      </c>
-      <c r="E4" s="9">
-        <v>11</v>
-      </c>
-      <c r="F4" s="31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="9">
-        <v>3</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="9">
-        <v>5</v>
-      </c>
-      <c r="E5" s="9">
-        <v>6</v>
-      </c>
-      <c r="F5" s="31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="9">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="D6" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="E6" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="F6" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9">
-        <v>5</v>
-      </c>
-      <c r="E7" s="9">
-        <v>11</v>
-      </c>
-      <c r="F7" s="31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="9">
-        <v>3</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="9">
-        <v>5</v>
-      </c>
-      <c r="E8" s="9">
-        <v>6</v>
-      </c>
-      <c r="F8" s="31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B9" s="9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="D9" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="E9" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="F9" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="C10" s="9">
-        <v>2</v>
-      </c>
-      <c r="D10" s="9">
-        <v>5</v>
-      </c>
-      <c r="E10" s="9">
-        <v>11</v>
-      </c>
-      <c r="F10" s="31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="9">
-        <v>3</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="9">
-        <v>5</v>
-      </c>
-      <c r="E11" s="9">
-        <v>6</v>
-      </c>
-      <c r="F11" s="31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="9">
-        <v>3</v>
-      </c>
-      <c r="C12" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="D12" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="E12" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="F12" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="C13" s="9">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9">
-        <v>5</v>
-      </c>
-      <c r="E13" s="9">
-        <v>11</v>
-      </c>
-      <c r="F13" s="31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="9">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="9">
-        <v>5</v>
-      </c>
-      <c r="E14" s="9">
-        <v>6</v>
-      </c>
-      <c r="F14" s="31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="9">
-        <v>3</v>
-      </c>
-      <c r="C15" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="D15" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="E15" s="9">
-        <v>12.5</v>
-      </c>
-      <c r="F15" s="31">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="114" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="98">
-        <v>2.5</v>
-      </c>
-      <c r="C16" s="98">
-        <v>2</v>
-      </c>
-      <c r="D16" s="98">
-        <v>5</v>
-      </c>
-      <c r="E16" s="98">
-        <v>11</v>
-      </c>
-      <c r="F16" s="102">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="9">
-        <v>3</v>
-      </c>
-      <c r="C17" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="D17" s="9">
-        <v>5</v>
-      </c>
-      <c r="E17" s="9">
-        <v>6</v>
-      </c>
-      <c r="F17" s="31">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="9">
-        <v>3.5</v>
-      </c>
-      <c r="C18" s="9">
-        <v>2</v>
-      </c>
-      <c r="D18" s="9">
-        <v>4.5</v>
-      </c>
-      <c r="E18" s="9">
-        <v>5</v>
-      </c>
-      <c r="F18" s="31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="10">
-        <v>8</v>
-      </c>
-      <c r="C19" s="10">
-        <v>6</v>
-      </c>
-      <c r="D19" s="10">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10">
-        <v>2</v>
-      </c>
-      <c r="F19" s="11">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -37621,6 +37295,393 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="9">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D3" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E3" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="F3" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>11</v>
+      </c>
+      <c r="F4" s="31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>6</v>
+      </c>
+      <c r="F5" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="F6" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>11</v>
+      </c>
+      <c r="F7" s="31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="9">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>6</v>
+      </c>
+      <c r="F8" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D9" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="F9" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2</v>
+      </c>
+      <c r="D10" s="9">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9">
+        <v>11</v>
+      </c>
+      <c r="F10" s="31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="9">
+        <v>5</v>
+      </c>
+      <c r="E11" s="9">
+        <v>6</v>
+      </c>
+      <c r="F11" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="9">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="F12" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="D13" s="9">
+        <v>5</v>
+      </c>
+      <c r="E13" s="9">
+        <v>11</v>
+      </c>
+      <c r="F13" s="31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9">
+        <v>6</v>
+      </c>
+      <c r="F14" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="9">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D15" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="E15" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="F15" s="31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="114" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="98">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="98">
+        <v>2</v>
+      </c>
+      <c r="D16" s="98">
+        <v>5</v>
+      </c>
+      <c r="E16" s="98">
+        <v>11</v>
+      </c>
+      <c r="F16" s="102">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="9">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="D17" s="9">
+        <v>5</v>
+      </c>
+      <c r="E17" s="9">
+        <v>6</v>
+      </c>
+      <c r="F17" s="31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="D18" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="E18" s="9">
+        <v>5</v>
+      </c>
+      <c r="F18" s="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="10">
+        <v>8</v>
+      </c>
+      <c r="C19" s="10">
+        <v>6</v>
+      </c>
+      <c r="D19" s="10">
+        <v>4</v>
+      </c>
+      <c r="E19" s="10">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E5CD4B-C8DB-4A49-956D-761D45563331}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -37716,7 +37777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982C988E-F277-4EB8-BD08-045871CAA4ED}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -37769,7 +37830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344AC655-401B-435E-9F3E-B4AFCEDA07DB}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -37842,7 +37903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F26805-7F3D-4935-8D0C-80B2E9E9F409}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -37895,7 +37956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D3944-A6F1-468B-A756-A99C077811C6}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -38185,7 +38246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6DB070-53D7-4763-B1D6-04233A007F0E}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -38290,7 +38351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C902C13-E391-4A34-8851-63FF84EE5034}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -38335,7 +38396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE67BAE-6607-47A3-AB16-0544FAF51C24}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -44463,7 +44524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD7B182-CFB4-4537-B5F7-69962DD30DA1}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -44576,7 +44637,56 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABFF4F0-1521-4984-985F-ECB7FE3DE71E}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BBCD48-6980-4EA6-BF3E-79D1C64EA04C}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -44637,56 +44747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ABFF4F0-1521-4984-985F-ECB7FE3DE71E}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:P3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805632D3-BD42-4D5C-8C0F-68DF124ED3E8}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -44747,7 +44808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D674F75E-153D-40A1-94D4-31ED20AACD7B}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -44918,7 +44979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCFBAE5B-BDCC-4DEB-A724-3B0573940C90}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45087,7 +45148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5996B071-C07A-46F0-B343-7584DB2F1269}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45146,7 +45207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE80B7E4-4C81-4B91-B37B-915E590A92F2}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45213,7 +45274,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823AFEBC-B792-4B8A-886B-A98A6A68E8F9}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45240,7 +45301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6590066-9C40-4D54-9CAB-C4CFCBEB3031}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45267,7 +45328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2338A37-BF8E-46F2-AA7C-FB95F874D0FC}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45326,7 +45387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EDDE38-2D71-4494-ABC1-8D5269A138D9}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45400,7 +45461,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682853F4-72D8-4EF0-AA50-363CCA43D5C1}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2F8796-71C2-44EA-9373-5A0165D7B559}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -45451,60 +45543,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AADDC2-B2BB-401C-A679-13FE5CA73888}">
   <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
+    <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>134</v>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="133">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134045F2-617D-4B6C-9AE3-C6E73CF3B321}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -45676,7 +45767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE4BAFD-2A94-4164-976F-B9E5B42E5AAB}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -45738,7 +45829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA334136-9628-4654-B8E2-BCFE701B0D1B}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -45791,7 +45882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF02372-561D-40F0-A559-919B07A104BB}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46080,7 +46171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFFE531-B1A6-4FB1-B54F-4F29B07D584D}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46172,7 +46263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB6A12E-8B05-4366-A90E-CF297972EC8F}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46242,7 +46333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE98AFE6-8AD4-4F61-8FD9-8C39A28FF436}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -46285,7 +46376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64191092-61FC-49E2-8B87-F024EB93CA2E}">
   <sheetPr>
     <tabColor theme="0"/>

</xml_diff>

<commit_message>
Fix header in WellPressure tab for strategic model input files
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFDA91F-B454-47D0-9444-505E19200729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17C1375-E45A-4AE5-9E30-56E0F57202F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3438" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="314">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1042,9 +1042,6 @@
   </si>
   <si>
     <t>max_allowable_pressure</t>
-  </si>
-  <si>
-    <t>Table of Production Rate Forecasts by Pads [bbl/day]</t>
   </si>
   <si>
     <t>Treatment Sites to Beneficial Reuse Piping Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
@@ -6758,7 +6755,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -6869,7 +6866,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7359,7 +7356,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7434,7 +7431,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7584,7 +7581,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -7679,7 +7676,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7730,7 +7727,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8647,7 +8644,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8719,7 +8716,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8769,7 +8766,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8810,7 +8807,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13148,7 +13145,7 @@
   <dimension ref="A1:BC23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13161,8 +13158,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>302</v>
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT("Well pressure at production or completions pad [",VLOOKUP("pressure", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Well pressure at production or completions pad [psi]</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>296</v>
@@ -46313,7 +46311,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B3" s="131">
         <v>0.2</v>

</xml_diff>

<commit_message>
Add all seismisity tabs to all strategic model input files
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17C1375-E45A-4AE5-9E30-56E0F57202F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653C9CC3-F8C6-4F51-9C0C-75EBA794995E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -110,6 +110,14 @@
     <sheet name="StorageExpansionLeadTime" sheetId="131" r:id="rId95"/>
     <sheet name="PipelineExpansionLeadTime_Dist" sheetId="132" r:id="rId96"/>
     <sheet name="PipelineExpansionLeadTime_Capac" sheetId="133" r:id="rId97"/>
+    <sheet name="SWDDeep" sheetId="139" r:id="rId98"/>
+    <sheet name="SWDAveragePressure" sheetId="140" r:id="rId99"/>
+    <sheet name="SWDProxPAWell" sheetId="141" r:id="rId100"/>
+    <sheet name="SWDProxInactiveWell" sheetId="142" r:id="rId101"/>
+    <sheet name="SWDProxEQ" sheetId="143" r:id="rId102"/>
+    <sheet name="SWDProxFault" sheetId="144" r:id="rId103"/>
+    <sheet name="SWDProxHpOrLpWell" sheetId="145" r:id="rId104"/>
+    <sheet name="SWDRiskFactors" sheetId="146" r:id="rId105"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
@@ -136,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3461" uniqueCount="335">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1079,6 +1087,69 @@
   <si>
     <t>Treatment Sites to Disposal Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
   </si>
+  <si>
+    <t>SWDs - shallow (0) or deep (1)</t>
+  </si>
+  <si>
+    <t>Average pressure/depth in vicinity of well [psi/ft]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to P&amp;A'd well [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to inactive/temporarily abandoned formerly producing well (completed prior to 2000) [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to earthquakes &gt;= 3.0 magnitude [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to fault [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to high pressure or low pressure injection well [miles]</t>
+  </si>
+  <si>
+    <t>SWD risk factors</t>
+  </si>
+  <si>
+    <t>orphan_well_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>orphan_well_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>inactive_well_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>inactive_well_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>EQ_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>EQ_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>fault_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>fault_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_LP_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_LP_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_threshold</t>
+  </si>
+  <si>
+    <t>psi/ft</t>
+  </si>
+  <si>
+    <t>LP_threshold</t>
+  </si>
 </sst>
 </file>
 
@@ -1701,7 +1772,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2006,6 +2077,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3050,6 +3143,286 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C1C72C-FA2D-415C-8B01-36FA63337895}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685D431B-18F2-4461-8FC6-A29F2FC5FE23}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EEC73E-D6E2-487A-A2DB-930BB8939764}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556972C4-5663-4A73-9E9A-FF3E8B0F5B25}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0983EAD-864E-4569-8B46-DC1E200F915E}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D3B522-462D-4325-824D-2B66A4ABA069}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="132" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="135" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="133"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="136" t="s">
+        <v>322</v>
+      </c>
+      <c r="B3" s="137">
+        <v>1.86</v>
+      </c>
+      <c r="C3" s="133"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="136" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" s="137">
+        <v>2</v>
+      </c>
+      <c r="C4" s="133"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="136" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" s="137">
+        <v>1.86</v>
+      </c>
+      <c r="C5" s="133"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="136" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" s="137">
+        <v>2</v>
+      </c>
+      <c r="C6" s="133"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="136" t="s">
+        <v>326</v>
+      </c>
+      <c r="B7" s="137">
+        <v>5.59</v>
+      </c>
+      <c r="C7" s="133"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="136" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="137">
+        <v>1</v>
+      </c>
+      <c r="C8" s="133"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="136" t="s">
+        <v>328</v>
+      </c>
+      <c r="B9" s="137">
+        <v>5.59</v>
+      </c>
+      <c r="C9" s="133"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="136" t="s">
+        <v>329</v>
+      </c>
+      <c r="B10" s="137">
+        <v>1</v>
+      </c>
+      <c r="C10" s="133"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="136" t="s">
+        <v>330</v>
+      </c>
+      <c r="B11" s="137">
+        <v>1.86</v>
+      </c>
+      <c r="C11" s="133"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="136" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" s="137">
+        <v>2</v>
+      </c>
+      <c r="C12" s="133"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="136" t="s">
+        <v>332</v>
+      </c>
+      <c r="B13" s="137">
+        <v>0.7</v>
+      </c>
+      <c r="C13" s="133" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="138" t="s">
+        <v>334</v>
+      </c>
+      <c r="B14" s="139">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="133" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C820352-28DB-4692-BCE8-9A9846CC4956}">
   <sheetPr>
@@ -46430,4 +46803,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F529B0B-6059-4A0E-ABAB-10B47FB80033}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C155BC-F83A-4EEC-B7B3-A05CB25D767F}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation updates for 1.0
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F05DCD-D32D-4253-91AC-2DC8B0993CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEFCE87-CFA4-4AF7-8C6B-C0F145B09904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2367,43 +2367,60 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>427181</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>11546</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>599823</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>54016</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC643757-8A56-DABF-6190-C867780BD2F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B97B5F8-DE22-7BDB-D1A5-7C96F69A040B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="427181" y="381001"/>
-          <a:ext cx="13045824" cy="5030106"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15601950" cy="6429375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4274,7 +4291,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4851,7 +4868,7 @@
   </sheetPr>
   <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13903,8 +13920,8 @@
   </sheetPr>
   <dimension ref="A1:BA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Documentation updates for 1.0 (#338)
* Documentation updates for 1.0

* Adjust size of image

(cherry picked from commit 068e70df2d9c95a10bdbb9a5f2e508c308be279e)
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_permian_demo.xlsx
+++ b/pareto/case_studies/strategic_permian_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F05DCD-D32D-4253-91AC-2DC8B0993CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEFCE87-CFA4-4AF7-8C6B-C0F145B09904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="929" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -2367,43 +2367,60 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>427181</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>11546</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>599823</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>54016</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC643757-8A56-DABF-6190-C867780BD2F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B97B5F8-DE22-7BDB-D1A5-7C96F69A040B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="427181" y="381001"/>
-          <a:ext cx="13045824" cy="5030106"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15601950" cy="6429375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -4274,7 +4291,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4851,7 +4868,7 @@
   </sheetPr>
   <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13903,8 +13920,8 @@
   </sheetPr>
   <dimension ref="A1:BA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>